<commit_message>
xlswrite - filtro por condición
</commit_message>
<xml_diff>
--- a/xlswrite/xls/filtros.xlsx
+++ b/xlswrite/xls/filtros.xlsx
@@ -7,20 +7,17 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Ficha con filtros" sheetId="1" r:id="rId1"/>
+    <sheet name="Ficha con filtros por condición" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ficha con filtros'!$B$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ficha con filtros por condición'!$A$1:$D$10</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>#</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nombre</t>
   </si>
@@ -32,9 +29,6 @@
   </si>
   <si>
     <t>Nota 3</t>
-  </si>
-  <si>
-    <t>Promedio</t>
   </si>
   <si>
     <t>Wilder Lizama</t>
@@ -403,18 +397,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="6" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="4" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,198 +420,138 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" hidden="1">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
         <v>8</v>
       </c>
-      <c r="D2">
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
         <v>5</v>
       </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3">
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>6.333333333333333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>6.666666666666667</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <v>6</v>
-      </c>
-      <c r="F6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
+      <c r="B7">
+        <v>9</v>
       </c>
       <c r="C7">
         <v>9</v>
       </c>
       <c r="D7">
-        <v>9</v>
-      </c>
-      <c r="E7">
-        <v>6</v>
-      </c>
-      <c r="F7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" hidden="1">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
+      <c r="D9">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="F8">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9">
-        <v>7</v>
-      </c>
-      <c r="F9">
-        <v>6.666666666666667</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <v>6</v>
-      </c>
-      <c r="E10">
-        <v>4</v>
-      </c>
-      <c r="F10">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="B1:F1">
-    <filterColumn colId="0">
+  <autoFilter ref="A1:D10">
+    <filterColumn colId="2">
       <customFilters>
-        <customFilter val="Oscan*"/>
+        <customFilter operator="greaterThan" val="5"/>
       </customFilters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
xlswrite - filtros con lista
</commit_message>
<xml_diff>
--- a/xlswrite/xls/filtros.xlsx
+++ b/xlswrite/xls/filtros.xlsx
@@ -8,8 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="Ficha con filtros por condición" sheetId="1" r:id="rId1"/>
+    <sheet name="Ficha con filtros de lista" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Ficha con filtros de lista'!$A$1:$B$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ficha con filtros por condición'!$A$1:$D$10</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Nombre</t>
   </si>
@@ -56,6 +58,48 @@
   </si>
   <si>
     <t>Kiori hayutaru</t>
+  </si>
+  <si>
+    <t>Nro. Mes</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Junio</t>
+  </si>
+  <si>
+    <t>Julio</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Septiembre</t>
+  </si>
+  <si>
+    <t>Octubre</t>
+  </si>
+  <si>
+    <t>Noviembre</t>
+  </si>
+  <si>
+    <t>Diciembre</t>
   </si>
 </sst>
 </file>
@@ -557,4 +601,135 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" hidden="1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" hidden="1">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" hidden="1">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" hidden="1">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" hidden="1">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" hidden="1">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" hidden="1">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" hidden="1">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" hidden="1">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B13">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="4"/>
+        <filter val="8"/>
+        <filter val="11"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>